<commit_message>
optimizations for paral & vect
</commit_message>
<xml_diff>
--- a/docs/вычислительные эксперименты.xlsx
+++ b/docs/вычислительные эксперименты.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Users\admin\Documents\discords_discovery\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5875F55A-E153-4B61-81A3-A1358D48FD0A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE1F5F7-2904-4F6A-AD56-B9554BAEB265}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17490" windowHeight="7995" xr2:uid="{45C03163-AE80-4B21-B1B4-A61EF55A8E8E}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
   <si>
     <t>Количество нитей</t>
   </si>
@@ -236,16 +237,16 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -257,19 +258,19 @@
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.630888</c:v>
+                  <c:v>0.30491299999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.23409099999999999</c:v>
+                  <c:v>0.2412765</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.30137049999999999</c:v>
+                  <c:v>0.21633200000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.30704200000000004</c:v>
+                  <c:v>0.3428465</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.36302899999999999</c:v>
+                  <c:v>0.60404749999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -568,16 +569,16 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -592,16 +593,16 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.6950544873574809</c:v>
+                  <c:v>1.2637492669199031</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0933966662297738</c:v>
+                  <c:v>1.4094678549636668</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.0547286690420199</c:v>
+                  <c:v>0.88935719046278727</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.7378446350016115</c:v>
+                  <c:v>0.50478315033172061</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -905,16 +906,16 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -929,16 +930,16 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.3475272436787404</c:v>
+                  <c:v>0.42124975563996769</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.52334916655744346</c:v>
+                  <c:v>0.23491130916061112</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.25684108363025249</c:v>
+                  <c:v>7.4113099205232277E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.10861528968760072</c:v>
+                  <c:v>2.8043508351762256E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -947,6 +948,1015 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-BE0E-4019-B385-E422BC6F8585}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="666119184"/>
+        <c:axId val="666119512"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="666119184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="666119512"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="666119512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="666119184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ru-RU"/>
+              <a:t>Зависимость "время-количество нитей"</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.18168044619422571"/>
+          <c:y val="4.6641986915814629E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист1!$C$4:$G$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист1!$C$9:$G$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.30491299999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2412765</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.21633200000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3428465</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.60404749999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B0C3-410C-99EE-87710E077DB5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="261502344"/>
+        <c:axId val="261502672"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="261502344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="261502672"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="261502672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="261502344"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ru-RU"/>
+              <a:t>Зависимость "ускорение-количество нитей"</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист1!$C$4:$G$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист1!$C$10:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2637492669199031</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.4094678549636668</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.88935719046278727</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.50478315033172061</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E3E7-459C-A154-3EFD063E8A32}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="261557104"/>
+        <c:axId val="324620928"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="261557104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="324620928"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="324620928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="261557104"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="ru-RU"/>
+              <a:t>Зависимость</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ru-RU" baseline="0"/>
+              <a:t> "эффективность-количество нитей</a:t>
+            </a:r>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Лист1!$C$4:$G$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Лист1!$C$11:$G$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.42124975563996769</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.23491130916061112</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.4113099205232277E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.8043508351762256E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B465-4DCF-B045-C2123FB1123A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1257,6 +2267,126 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2290,6 +3420,1554 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2902,6 +5580,125 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Диаграмма 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A23526D-022D-4D68-B534-CB7743425F76}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Диаграмма 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{514142F3-147B-4149-BE42-90CFAE2E9208}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Диаграмма 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75E5F81A-7ECA-4DCA-87AF-E51616246A77}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -3215,10 +6012,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{820E519F-FAA0-49C3-93F6-DD03DB762C1A}">
-  <dimension ref="B3:G11"/>
+  <dimension ref="B3:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3226,7 +6023,7 @@
     <col min="2" max="2" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="C3" s="5" t="s">
         <v>0</v>
@@ -3236,7 +6033,7 @@
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
@@ -3244,124 +6041,143 @@
         <v>1</v>
       </c>
       <c r="D4" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E4" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F4" s="2">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G4" s="2">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="H4" s="2">
+        <v>24</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>1</v>
       </c>
       <c r="C5" s="2">
-        <v>0.30615100000000001</v>
+        <v>0.25486599999999998</v>
       </c>
       <c r="D5" s="2">
-        <v>0.26847599999999999</v>
+        <v>0.194665</v>
       </c>
       <c r="E5" s="2">
-        <v>0.17841899999999999</v>
+        <v>0.24160200000000001</v>
       </c>
       <c r="F5" s="2">
-        <v>0.25877800000000001</v>
+        <v>0.36257600000000001</v>
       </c>
       <c r="G5" s="2">
-        <v>0.41499599999999998</v>
+        <v>0.78539700000000001</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.77568499999999996</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>2</v>
       </c>
       <c r="C6" s="2">
-        <v>0.72289899999999996</v>
+        <v>0.27200099999999999</v>
       </c>
       <c r="D6" s="2">
-        <v>0.19970599999999999</v>
+        <v>0.45183499999999999</v>
       </c>
       <c r="E6" s="2">
-        <v>0.332179</v>
+        <v>0.26638800000000001</v>
       </c>
       <c r="F6" s="2">
-        <v>0.33150200000000002</v>
+        <v>0.34936699999999998</v>
       </c>
       <c r="G6" s="2">
-        <v>0.31820399999999999</v>
+        <v>0.298788</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.69952899999999996</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <v>3</v>
       </c>
       <c r="C7" s="2">
-        <v>0.98431999999999997</v>
+        <v>0.33782499999999999</v>
       </c>
       <c r="D7" s="2">
-        <v>0.18548500000000001</v>
+        <v>0.215365</v>
       </c>
       <c r="E7" s="2">
-        <v>0.51480199999999998</v>
+        <v>0.19106200000000001</v>
       </c>
       <c r="F7" s="2">
-        <v>0.49763800000000002</v>
+        <v>0.33632600000000001</v>
       </c>
       <c r="G7" s="2">
-        <v>0.40785399999999999</v>
+        <v>0.66907799999999995</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0.46202199999999999</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <v>4</v>
       </c>
       <c r="C8" s="2">
-        <v>0.53887700000000005</v>
+        <v>0.44090600000000002</v>
       </c>
       <c r="D8" s="2">
-        <v>0.40944700000000001</v>
+        <v>0.26718799999999998</v>
       </c>
       <c r="E8" s="2">
-        <v>0.27056200000000002</v>
+        <v>0.189112</v>
       </c>
       <c r="F8" s="2">
-        <v>0.282582</v>
+        <v>0.28564800000000001</v>
       </c>
       <c r="G8" s="2">
-        <v>0.273345</v>
+        <v>0.53901699999999997</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0.30650899999999998</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C9" s="3">
         <f>MEDIAN(C5:C8)</f>
-        <v>0.630888</v>
+        <v>0.30491299999999999</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" ref="D9:G9" si="0">MEDIAN(D5:D8)</f>
-        <v>0.23409099999999999</v>
+        <v>0.2412765</v>
       </c>
       <c r="E9" s="3">
         <f t="shared" si="0"/>
-        <v>0.30137049999999999</v>
+        <v>0.21633200000000002</v>
       </c>
       <c r="F9" s="3">
         <f t="shared" si="0"/>
-        <v>0.30704200000000004</v>
+        <v>0.3428465</v>
       </c>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
-        <v>0.36302899999999999</v>
+        <v>0.60404749999999996</v>
+      </c>
+      <c r="H9" s="3">
+        <f t="shared" ref="H9" si="1">MEDIAN(H5:H8)</f>
+        <v>0.5807755</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>1</v>
       </c>
@@ -3370,23 +6186,27 @@
         <v>1</v>
       </c>
       <c r="D10" s="4">
-        <f t="shared" ref="D10:G10" si="1">$C9/D9</f>
-        <v>2.6950544873574809</v>
+        <f t="shared" ref="D10:G10" si="2">$C9/D9</f>
+        <v>1.2637492669199031</v>
       </c>
       <c r="E10" s="4">
-        <f t="shared" si="1"/>
-        <v>2.0933966662297738</v>
+        <f t="shared" si="2"/>
+        <v>1.4094678549636668</v>
       </c>
       <c r="F10" s="4">
-        <f t="shared" si="1"/>
-        <v>2.0547286690420199</v>
+        <f t="shared" si="2"/>
+        <v>0.88935719046278727</v>
       </c>
       <c r="G10" s="4">
-        <f t="shared" si="1"/>
-        <v>1.7378446350016115</v>
+        <f t="shared" si="2"/>
+        <v>0.50478315033172061</v>
+      </c>
+      <c r="H10" s="4">
+        <f t="shared" ref="H10" si="3">$C9/H9</f>
+        <v>0.52501009426189638</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>2</v>
       </c>
@@ -3395,20 +6215,24 @@
         <v>1</v>
       </c>
       <c r="D11" s="2">
-        <f t="shared" ref="D11:G11" si="2">D10/D4</f>
-        <v>1.3475272436787404</v>
+        <f t="shared" ref="D11:G11" si="4">D10/D4</f>
+        <v>0.42124975563996769</v>
       </c>
       <c r="E11" s="2">
-        <f t="shared" si="2"/>
-        <v>0.52334916655744346</v>
+        <f t="shared" si="4"/>
+        <v>0.23491130916061112</v>
       </c>
       <c r="F11" s="2">
-        <f t="shared" si="2"/>
-        <v>0.25684108363025249</v>
+        <f t="shared" si="4"/>
+        <v>7.4113099205232277E-2</v>
       </c>
       <c r="G11" s="2">
-        <f t="shared" si="2"/>
-        <v>0.10861528968760072</v>
+        <f t="shared" si="4"/>
+        <v>2.8043508351762256E-2</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" ref="H11" si="5">H10/H4</f>
+        <v>2.1875420594245683E-2</v>
       </c>
     </row>
   </sheetData>
@@ -3419,4 +6243,235 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C2C2CD3-B565-4B90-AEB5-FD10A4BB0677}">
+  <dimension ref="B3:H11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:R34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="2"/>
+      <c r="C3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2">
+        <v>6</v>
+      </c>
+      <c r="F4" s="2">
+        <v>12</v>
+      </c>
+      <c r="G4" s="2">
+        <v>18</v>
+      </c>
+      <c r="H4" s="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.25486599999999998</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.194665</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.24160200000000001</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.36257600000000001</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0.78539700000000001</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.77568499999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="2">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.27200099999999999</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.45183499999999999</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.26638800000000001</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.34936699999999998</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.298788</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.69952899999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="2">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.33782499999999999</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.215365</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.19106200000000001</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.33632600000000001</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0.66907799999999995</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0.46202199999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="2">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.44090600000000002</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.26718799999999998</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.189112</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.28564800000000001</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.53901699999999997</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0.30650899999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="3">
+        <f>MEDIAN(C5:C8)</f>
+        <v>0.30491299999999999</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" ref="D9:H9" si="0">MEDIAN(D5:D8)</f>
+        <v>0.2412765</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" si="0"/>
+        <v>0.21633200000000002</v>
+      </c>
+      <c r="F9" s="3">
+        <f t="shared" si="0"/>
+        <v>0.3428465</v>
+      </c>
+      <c r="G9" s="3">
+        <f t="shared" si="0"/>
+        <v>0.60404749999999996</v>
+      </c>
+      <c r="H9" s="3">
+        <f t="shared" si="0"/>
+        <v>0.5807755</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="4">
+        <f>$C9/C9</f>
+        <v>1</v>
+      </c>
+      <c r="D10" s="4">
+        <f t="shared" ref="D10:H10" si="1">$C9/D9</f>
+        <v>1.2637492669199031</v>
+      </c>
+      <c r="E10" s="4">
+        <f t="shared" si="1"/>
+        <v>1.4094678549636668</v>
+      </c>
+      <c r="F10" s="4">
+        <f t="shared" si="1"/>
+        <v>0.88935719046278727</v>
+      </c>
+      <c r="G10" s="4">
+        <f t="shared" si="1"/>
+        <v>0.50478315033172061</v>
+      </c>
+      <c r="H10" s="4">
+        <f t="shared" si="1"/>
+        <v>0.52501009426189638</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="2">
+        <f>C10/C4</f>
+        <v>1</v>
+      </c>
+      <c r="D11" s="2">
+        <f t="shared" ref="D11:H11" si="2">D10/D4</f>
+        <v>0.42124975563996769</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="2"/>
+        <v>0.23491130916061112</v>
+      </c>
+      <c r="F11" s="2">
+        <f t="shared" si="2"/>
+        <v>7.4113099205232277E-2</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="2"/>
+        <v>2.8043508351762256E-2</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="2"/>
+        <v>2.1875420594245683E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C3:G3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>